<commit_message>
fix: original import templates
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/default time logs format.xlsx
+++ b/AccuPay/ImportTemplates/default time logs format.xlsx
@@ -35,7 +35,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -69,7 +69,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,7 +352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>